<commit_message>
java utility committed Signed-off-by: Sanjot <sanjotr16@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15870" windowHeight="4380"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:L13"/>
 </workbook>
 </file>
 
@@ -425,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -530,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
commit done on 28th june
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15870" windowHeight="4380"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15870" windowHeight="3750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L13"/>
+  <oleSize ref="D1:R11"/>
 </workbook>
 </file>
 
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>